<commit_message>
add new exercises, fix typo, update anki deck/wordlist
- fixed a typo in lesson-17/vocab-6; あまり短くじゃないでください --> あまり短くしないでください. (2nd ed.)
- updated anki deck/wordlist for Lesson 17 with useful exp. vocab. (3rd ed.)
- added the following exercises.

# Lesson 17 (3rd ed.)
- Useful Expressions: At the Hair Salon
- Useful Expressions: Hair Salon Words
- Workbook: ～そうです (I hear)／～って
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-17.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-17.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1129,6 +1129,306 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>I would like to have my hair cut.</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>カットをお願いします。|カットをおねがいします。</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Please don't make it too short.</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>あまり短くしないでください。|あまりみじかくしないでください。</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Please don't shave me.</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>そらないでください。</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Please cut off about 3 centimeters.</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>３センチぐらい切ってください。|３センチぐらいきってください。</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Please cut the back all the same length.</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>後ろをそろえてください。|うしろをそろえてください。</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Please dye my hair red.</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>赤にそめてください。|あかにそめてください。</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>I want my hair to be like Bob Marley's.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ボブ・マーリーみたいな髪形にしたいんですが。|ボブ・マーリーみたいなかみがたにしたいんですが。</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>shampoo</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>シャンプー</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>cut</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>カット</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>blow-dry</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ブロー</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>パーマ</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>hair coloring</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>カラー</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>set</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>セット</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>hair style</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>髪形|かみがた</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>to cut</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>切る|きる</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>to shave</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>そる</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>to crop</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>刈る|かる</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>to dye</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>そめる</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>to make hair even; to trim</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>そろえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>to have one's hair permed</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>パーマをかける</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>to thin out (hair)</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>すく</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>parting (of the hair)</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>分け目|わけめ</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>bangs</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>前髪|まえがみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>side</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>横|よこ</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>back</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>後ろ|うしろ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add new exercises, update anki decks/wordlists
- updated anki deck/wordlist for Lesson 17 with Kanji Vocabulary. (3rd ed.)
- added the following exercises.

# Lesson 17 (3rd ed.)
- Kanji Vocabulary: 野, 習, and 主
- Kanji Vocabulary: 歳, 集, and 発
- Kanji Vocabulary: 表, 品, and 写
- Kanji Vocabulary: 真, 字, and 活
- Kanji Vocabulary: 結, 婚, and 歩
- Kanji Practice: Write the Readings
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-17.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-17.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1429,6 +1429,774 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>realm; field</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>分野|ぶんや</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Mr./Ms. Ono</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>小野さん|おのさん</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Nagano</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>長野|ながの</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>baseball</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>野球|やきゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>vegetable</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>野菜|やさい</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>to learn</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>習う|ならう</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>calligraphy</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>習字|しゅうじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>practice</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>練習|れんしゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>habit; custom</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>習慣|しゅうかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>mainly</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>主に|おもに</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>husband</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>ご主人|ごしゅじん</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>housewife</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>主婦|しゅふ</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>subject of a sentence</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>主語|しゅご</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>持ち主|もちぬし</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>twenty-five years old</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>二十五歳|にじゅうごさい</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>year-end gift</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>お歳暮|おせいぼ</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>twenty years old</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>二十歳|はたち</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>to collect</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>集める|あつめる</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>(magazine) feature</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>特集|とくしゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>to concentrate</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>集中する|しゅうちゅうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>to make public; to give a presentation</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>発表する|はっぴょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>pronunciation</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>発音|はつおん</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>departure</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>出発|しゅっぱつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>invention</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>発明|はつめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>to make public; to give a presentation</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>発表する|はっぴょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>cover page</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>表紙|ひょうし</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>expression</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>表現|ひょうげん</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>to express</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>表す|あらわす</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>the front</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>表|おもて</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>work (of art, etc.)</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>作品|さくひん</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>elegant</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>上品な|じょうひんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>magic</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>手品|てじな</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>article of merchandise</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>品物|しなもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>photograph</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>写真|しゃしん</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>to copy</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>写す|うつす</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>sketch</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>写生|しゃせい</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>to describe</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>描写する|びょうしゃする</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>photograph</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>写真|しゃしん</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>center</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>真ん中|まんなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>right above...</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>～の真上|～のまうえ</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>midnight</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>真夜中|まよなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>character</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>文字|もじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>deficit</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>赤字|あかじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>family name</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>名字|みょうじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>uppercase letters</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>大文字|おおもじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Chinese character</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>漢字|かんじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>活動|かつどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>life; living</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>生活|せいかつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>活発な|かっぱつな</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>conjugation</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>活用|かつよう</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>liveliness</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>活気|かっき</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>to get married</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>結婚する|けっこんする</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>結果|けっか</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>conclusion</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>結論|けつろん</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>to tie a knot</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>結ぶ|むすぶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>divorce</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>離婚|りこん</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>fiancé(e)</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>婚約者|こんやくしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>newlywed</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>新婚|しんこん</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>unmarried</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>未婚|みこん</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>to walk</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>歩く|あるく</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>sidewalk</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>歩道|ほどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>to stroll</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>散歩する|さんぽする</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>one step</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>一歩|いっぽ</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>progress</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>進歩|しんぽ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>